<commit_message>
[Ballistic_Calculator] - Improved dragForce calculation. - Added ability to choose integration method (Euler or RK4). - Implemented drag model selection (G1, G7). - Added Gravity.py module to compute gravity acceleration. - Now results can be displays in the table. - Introduced settings for minimum velocity, altitude, and max distance. - Improved UI layout and parameter input structure. - Updated InterimWorkReport.pptx presentation accordingly.
</commit_message>
<xml_diff>
--- a/Ballistic_Calculator/Reporting/LiteratureReview.xlsx
+++ b/Ballistic_Calculator/Reporting/LiteratureReview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Algorithms_and_data_structures\Ballistic_Calculator\Reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F759B961-563A-49CE-AEB0-1D8B472D2F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A626B155-577B-40BE-81A9-0E283D6EE3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12330" yWindow="585" windowWidth="23160" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11790" yWindow="765" windowWidth="23160" windowHeight="20115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="155">
   <si>
     <t>Название</t>
   </si>
@@ -482,6 +482,18 @@
   </si>
   <si>
     <t>[24]</t>
+  </si>
+  <si>
+    <t>World Geodetic System (1984) // ahrs.readthedocs.io</t>
+  </si>
+  <si>
+    <t>[25]</t>
+  </si>
+  <si>
+    <t>(16.04.2025)</t>
+  </si>
+  <si>
+    <t>​Сайт предоставляет подробную информацию о модели WGS84 (World Geodetic System 1984), включая формулы для расчета нормального ускорения свободного падения на поверхности Земли и на высотах над ней.</t>
   </si>
 </sst>
 </file>
@@ -924,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,9 +1527,19 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="G26" s="17"/>
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>

</xml_diff>